<commit_message>
Fixed an error on the spreadsheet
</commit_message>
<xml_diff>
--- a/TheResultsData.xlsx
+++ b/TheResultsData.xlsx
@@ -56,12 +56,6 @@
     <t>Simulation Time: 50 minutes</t>
   </si>
   <si>
-    <t>Avg time new phone customer: 45 sec</t>
-  </si>
-  <si>
-    <t>Avg time new door customer: 55 sec</t>
-  </si>
-  <si>
     <t>Avg Time to answer  question: 24 seconds</t>
   </si>
   <si>
@@ -72,6 +66,12 @@
   </si>
   <si>
     <t>3000 seconds / 45 = 67</t>
+  </si>
+  <si>
+    <t>Avg time new door customer: 45 sec</t>
+  </si>
+  <si>
+    <t>Avg time new phone customer: 55 sec</t>
   </si>
 </sst>
 </file>
@@ -158,36 +158,39 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -475,7 +478,7 @@
   <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="I16" sqref="I16:J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -492,455 +495,523 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-    </row>
-    <row r="4" spans="1:14" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+    </row>
+    <row r="4" spans="1:14" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
     </row>
     <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="5" t="s">
+      <c r="B5" s="7"/>
+      <c r="C5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5" t="s">
+      <c r="D5" s="7"/>
+      <c r="E5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="6"/>
-      <c r="K5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="L5" s="6"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="7"/>
+      <c r="K5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L5" s="7"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
     </row>
     <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="7"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
+      <c r="A6" s="2"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9" t="s">
+      <c r="B7" s="12"/>
+      <c r="C7" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9" t="s">
+      <c r="D7" s="12"/>
+      <c r="E7" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9" t="s">
+      <c r="F7" s="12"/>
+      <c r="G7" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9" t="s">
+      <c r="H7" s="12"/>
+      <c r="I7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9" t="s">
+      <c r="J7" s="12"/>
+      <c r="K7" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="L7" s="9"/>
+      <c r="L7" s="12"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+      <c r="A8" s="10">
         <v>1</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1">
+      <c r="B8" s="10"/>
+      <c r="C8" s="10">
         <v>82</v>
       </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1">
+      <c r="D8" s="10"/>
+      <c r="E8" s="10">
         <v>42</v>
       </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1">
+      <c r="F8" s="10"/>
+      <c r="G8" s="10">
         <v>40</v>
       </c>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1">
+      <c r="H8" s="10"/>
+      <c r="I8" s="10">
         <v>43</v>
       </c>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1">
+      <c r="J8" s="10"/>
+      <c r="K8" s="10">
         <v>39</v>
       </c>
-      <c r="L8" s="1"/>
+      <c r="L8" s="10"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+      <c r="A9" s="10">
         <v>2</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1">
+      <c r="B9" s="10"/>
+      <c r="C9" s="10">
         <v>81</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1">
+      <c r="D9" s="10"/>
+      <c r="E9" s="10">
         <v>44</v>
       </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1">
+      <c r="F9" s="10"/>
+      <c r="G9" s="10">
         <v>37</v>
       </c>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1">
+      <c r="H9" s="10"/>
+      <c r="I9" s="10">
         <v>34</v>
       </c>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1">
+      <c r="J9" s="10"/>
+      <c r="K9" s="10">
         <v>47</v>
       </c>
-      <c r="L9" s="1"/>
+      <c r="L9" s="10"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+      <c r="A10" s="10">
         <v>3</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1">
+      <c r="B10" s="10"/>
+      <c r="C10" s="10">
         <v>72</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1">
+      <c r="D10" s="10"/>
+      <c r="E10" s="10">
         <v>46</v>
       </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1">
+      <c r="F10" s="10"/>
+      <c r="G10" s="10">
         <v>26</v>
       </c>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1">
+      <c r="H10" s="10"/>
+      <c r="I10" s="10">
         <v>33</v>
       </c>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1">
+      <c r="J10" s="10"/>
+      <c r="K10" s="10">
         <v>39</v>
       </c>
-      <c r="L10" s="1"/>
+      <c r="L10" s="10"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+      <c r="A11" s="10">
         <v>4</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1">
+      <c r="B11" s="10"/>
+      <c r="C11" s="10">
         <v>61</v>
       </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1">
+      <c r="D11" s="10"/>
+      <c r="E11" s="10">
         <v>41</v>
       </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1">
+      <c r="F11" s="10"/>
+      <c r="G11" s="10">
         <v>20</v>
       </c>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1">
+      <c r="H11" s="10"/>
+      <c r="I11" s="10">
         <v>31</v>
       </c>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1">
+      <c r="J11" s="10"/>
+      <c r="K11" s="10">
         <v>30</v>
       </c>
-      <c r="L11" s="1"/>
+      <c r="L11" s="10"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+      <c r="A12" s="10">
         <v>5</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1">
+      <c r="B12" s="10"/>
+      <c r="C12" s="10">
         <v>83</v>
       </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1">
+      <c r="D12" s="10"/>
+      <c r="E12" s="10">
         <v>42</v>
       </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1">
+      <c r="F12" s="10"/>
+      <c r="G12" s="10">
         <v>41</v>
       </c>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1">
+      <c r="H12" s="10"/>
+      <c r="I12" s="10">
         <v>37</v>
       </c>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1">
+      <c r="J12" s="10"/>
+      <c r="K12" s="10">
         <v>46</v>
       </c>
-      <c r="L12" s="1"/>
+      <c r="L12" s="10"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+      <c r="A13" s="10">
         <v>6</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1">
+      <c r="B13" s="10"/>
+      <c r="C13" s="10">
         <v>90</v>
       </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1">
+      <c r="D13" s="10"/>
+      <c r="E13" s="10">
         <v>45</v>
       </c>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1">
+      <c r="F13" s="10"/>
+      <c r="G13" s="10">
         <v>45</v>
       </c>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1">
+      <c r="H13" s="10"/>
+      <c r="I13" s="10">
         <v>41</v>
       </c>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1">
+      <c r="J13" s="10"/>
+      <c r="K13" s="10">
         <v>49</v>
       </c>
-      <c r="L13" s="1"/>
+      <c r="L13" s="10"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+      <c r="A14" s="10">
         <v>7</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1">
+      <c r="B14" s="10"/>
+      <c r="C14" s="10">
         <v>75</v>
       </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1">
+      <c r="D14" s="10"/>
+      <c r="E14" s="10">
         <v>40</v>
       </c>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1">
+      <c r="F14" s="10"/>
+      <c r="G14" s="10">
         <v>35</v>
       </c>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1">
+      <c r="H14" s="10"/>
+      <c r="I14" s="10">
         <v>35</v>
       </c>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1">
+      <c r="J14" s="10"/>
+      <c r="K14" s="10">
         <v>40</v>
       </c>
-      <c r="L14" s="1"/>
+      <c r="L14" s="10"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+      <c r="A15" s="10">
         <v>8</v>
       </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1">
+      <c r="B15" s="10"/>
+      <c r="C15" s="10">
         <v>66</v>
       </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1">
+      <c r="D15" s="10"/>
+      <c r="E15" s="10">
         <v>37</v>
       </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1">
+      <c r="F15" s="10"/>
+      <c r="G15" s="10">
         <v>29</v>
       </c>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1">
+      <c r="H15" s="10"/>
+      <c r="I15" s="10">
         <v>24</v>
       </c>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1">
+      <c r="J15" s="10"/>
+      <c r="K15" s="10">
         <v>42</v>
       </c>
-      <c r="L15" s="1"/>
+      <c r="L15" s="10"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+      <c r="A16" s="10">
         <v>9</v>
       </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1">
+      <c r="B16" s="10"/>
+      <c r="C16" s="10">
         <v>73</v>
       </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1">
+      <c r="D16" s="10"/>
+      <c r="E16" s="10">
         <v>43</v>
       </c>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1">
+      <c r="F16" s="10"/>
+      <c r="G16" s="10">
         <v>30</v>
       </c>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1">
+      <c r="H16" s="10"/>
+      <c r="I16" s="10">
         <v>29</v>
       </c>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1">
+      <c r="J16" s="10"/>
+      <c r="K16" s="10">
         <v>44</v>
       </c>
-      <c r="L16" s="1"/>
+      <c r="L16" s="10"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
+      <c r="A17" s="10">
         <v>10</v>
       </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1">
+      <c r="B17" s="10"/>
+      <c r="C17" s="10">
         <v>71</v>
       </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1">
+      <c r="D17" s="10"/>
+      <c r="E17" s="10">
         <v>41</v>
       </c>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1">
+      <c r="F17" s="10"/>
+      <c r="G17" s="10">
         <v>30</v>
       </c>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1">
+      <c r="H17" s="10"/>
+      <c r="I17" s="10">
         <v>31</v>
       </c>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1">
+      <c r="J17" s="10"/>
+      <c r="K17" s="10">
         <v>40</v>
       </c>
-      <c r="L17" s="1"/>
+      <c r="L17" s="10"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3">
+      <c r="B18" s="9"/>
+      <c r="C18" s="9">
         <f>SUM(C17,C16,C15,C14,C13,C12,C11,C10,C9,C8) / 10</f>
         <v>75.400000000000006</v>
       </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3">
+      <c r="D18" s="9"/>
+      <c r="E18" s="9">
         <f>SUM(E17,E16,E15,E14,E13,E12,E11,E10,E9,E8)/10</f>
         <v>42.1</v>
       </c>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3">
+      <c r="F18" s="9"/>
+      <c r="G18" s="9">
         <f>SUM(G8:H17)/10</f>
         <v>33.299999999999997</v>
       </c>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3">
+      <c r="H18" s="9"/>
+      <c r="I18" s="9">
         <f>SUM(I8:J17)/10</f>
         <v>33.799999999999997</v>
       </c>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3">
+      <c r="J18" s="9"/>
+      <c r="K18" s="9">
         <f>SUM(K8:L17)/10</f>
         <v>41.6</v>
       </c>
-      <c r="L18" s="3"/>
+      <c r="L18" s="9"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12">
+      <c r="A19" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8">
         <f>SUM(67+55)</f>
         <v>122</v>
       </c>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="L19" s="12"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J19" s="8"/>
+      <c r="K19" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="L19" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="84">
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="A1:L3"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="K17:L17"/>
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="K5:L5"/>
     <mergeCell ref="E5:H5"/>
@@ -957,74 +1028,6 @@
     <mergeCell ref="I18:J18"/>
     <mergeCell ref="K18:L18"/>
     <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="A1:L3"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G11:H11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
Changed the colors on the spreadsheet
</commit_message>
<xml_diff>
--- a/TheResultsData.xlsx
+++ b/TheResultsData.xlsx
@@ -115,12 +115,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -143,6 +137,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -156,47 +156,44 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
-    <cellStyle name="20% - Accent5" xfId="2" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="2" builtinId="47"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -478,7 +475,7 @@
   <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16:J16"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,52 +492,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
     </row>
@@ -561,28 +558,28 @@
       <c r="N4" s="4"/>
     </row>
     <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="6" t="s">
+      <c r="B5" s="10"/>
+      <c r="C5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="6" t="s">
+      <c r="D5" s="10"/>
+      <c r="E5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6" t="s">
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="7"/>
-      <c r="K5" s="6" t="s">
+      <c r="J5" s="10"/>
+      <c r="K5" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="L5" s="7"/>
+      <c r="L5" s="10"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
     </row>
@@ -603,368 +600,394 @@
       <c r="N6" s="1"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12" t="s">
+      <c r="B7" s="7"/>
+      <c r="C7" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12" t="s">
+      <c r="D7" s="7"/>
+      <c r="E7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12" t="s">
+      <c r="F7" s="7"/>
+      <c r="G7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12" t="s">
+      <c r="H7" s="7"/>
+      <c r="I7" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12" t="s">
+      <c r="J7" s="7"/>
+      <c r="K7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="L7" s="12"/>
+      <c r="L7" s="7"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="10">
+      <c r="A8" s="6">
         <v>1</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10">
+      <c r="B8" s="6"/>
+      <c r="C8" s="6">
         <v>82</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10">
+      <c r="D8" s="6"/>
+      <c r="E8" s="6">
         <v>42</v>
       </c>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10">
+      <c r="F8" s="6"/>
+      <c r="G8" s="6">
         <v>40</v>
       </c>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10">
+      <c r="H8" s="6"/>
+      <c r="I8" s="6">
         <v>43</v>
       </c>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10">
+      <c r="J8" s="6"/>
+      <c r="K8" s="6">
         <v>39</v>
       </c>
-      <c r="L8" s="10"/>
+      <c r="L8" s="6"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="10">
+      <c r="A9" s="6">
         <v>2</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10">
+      <c r="B9" s="6"/>
+      <c r="C9" s="6">
         <v>81</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10">
+      <c r="D9" s="6"/>
+      <c r="E9" s="6">
         <v>44</v>
       </c>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10">
+      <c r="F9" s="6"/>
+      <c r="G9" s="6">
         <v>37</v>
       </c>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10">
+      <c r="H9" s="6"/>
+      <c r="I9" s="6">
         <v>34</v>
       </c>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10">
+      <c r="J9" s="6"/>
+      <c r="K9" s="6">
         <v>47</v>
       </c>
-      <c r="L9" s="10"/>
+      <c r="L9" s="6"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="10">
+      <c r="A10" s="6">
         <v>3</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10">
+      <c r="B10" s="6"/>
+      <c r="C10" s="6">
         <v>72</v>
       </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10">
+      <c r="D10" s="6"/>
+      <c r="E10" s="6">
         <v>46</v>
       </c>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10">
+      <c r="F10" s="6"/>
+      <c r="G10" s="6">
         <v>26</v>
       </c>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10">
+      <c r="H10" s="6"/>
+      <c r="I10" s="6">
         <v>33</v>
       </c>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10">
+      <c r="J10" s="6"/>
+      <c r="K10" s="6">
         <v>39</v>
       </c>
-      <c r="L10" s="10"/>
+      <c r="L10" s="6"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="10">
+      <c r="A11" s="6">
         <v>4</v>
       </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10">
+      <c r="B11" s="6"/>
+      <c r="C11" s="6">
         <v>61</v>
       </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10">
+      <c r="D11" s="6"/>
+      <c r="E11" s="6">
         <v>41</v>
       </c>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10">
+      <c r="F11" s="6"/>
+      <c r="G11" s="6">
         <v>20</v>
       </c>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10">
+      <c r="H11" s="6"/>
+      <c r="I11" s="6">
         <v>31</v>
       </c>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10">
+      <c r="J11" s="6"/>
+      <c r="K11" s="6">
         <v>30</v>
       </c>
-      <c r="L11" s="10"/>
+      <c r="L11" s="6"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="10">
+      <c r="A12" s="6">
         <v>5</v>
       </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10">
+      <c r="B12" s="6"/>
+      <c r="C12" s="6">
         <v>83</v>
       </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10">
+      <c r="D12" s="6"/>
+      <c r="E12" s="6">
         <v>42</v>
       </c>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10">
+      <c r="F12" s="6"/>
+      <c r="G12" s="6">
         <v>41</v>
       </c>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10">
+      <c r="H12" s="6"/>
+      <c r="I12" s="6">
         <v>37</v>
       </c>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10">
+      <c r="J12" s="6"/>
+      <c r="K12" s="6">
         <v>46</v>
       </c>
-      <c r="L12" s="10"/>
+      <c r="L12" s="6"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="10">
+      <c r="A13" s="6">
         <v>6</v>
       </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10">
+      <c r="B13" s="6"/>
+      <c r="C13" s="6">
         <v>90</v>
       </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10">
+      <c r="D13" s="6"/>
+      <c r="E13" s="6">
         <v>45</v>
       </c>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10">
+      <c r="F13" s="6"/>
+      <c r="G13" s="6">
         <v>45</v>
       </c>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10">
+      <c r="H13" s="6"/>
+      <c r="I13" s="6">
         <v>41</v>
       </c>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10">
+      <c r="J13" s="6"/>
+      <c r="K13" s="6">
         <v>49</v>
       </c>
-      <c r="L13" s="10"/>
+      <c r="L13" s="6"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="10">
+      <c r="A14" s="6">
         <v>7</v>
       </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10">
+      <c r="B14" s="6"/>
+      <c r="C14" s="6">
         <v>75</v>
       </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10">
+      <c r="D14" s="6"/>
+      <c r="E14" s="6">
         <v>40</v>
       </c>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10">
+      <c r="F14" s="6"/>
+      <c r="G14" s="6">
         <v>35</v>
       </c>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10">
+      <c r="H14" s="6"/>
+      <c r="I14" s="6">
         <v>35</v>
       </c>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10">
+      <c r="J14" s="6"/>
+      <c r="K14" s="6">
         <v>40</v>
       </c>
-      <c r="L14" s="10"/>
+      <c r="L14" s="6"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="10">
+      <c r="A15" s="6">
         <v>8</v>
       </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10">
+      <c r="B15" s="6"/>
+      <c r="C15" s="6">
         <v>66</v>
       </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10">
+      <c r="D15" s="6"/>
+      <c r="E15" s="6">
         <v>37</v>
       </c>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10">
+      <c r="F15" s="6"/>
+      <c r="G15" s="6">
         <v>29</v>
       </c>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10">
+      <c r="H15" s="6"/>
+      <c r="I15" s="6">
         <v>24</v>
       </c>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10">
+      <c r="J15" s="6"/>
+      <c r="K15" s="6">
         <v>42</v>
       </c>
-      <c r="L15" s="10"/>
+      <c r="L15" s="6"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="10">
+      <c r="A16" s="6">
         <v>9</v>
       </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10">
+      <c r="B16" s="6"/>
+      <c r="C16" s="6">
         <v>73</v>
       </c>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10">
+      <c r="D16" s="6"/>
+      <c r="E16" s="6">
         <v>43</v>
       </c>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10">
+      <c r="F16" s="6"/>
+      <c r="G16" s="6">
         <v>30</v>
       </c>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10">
+      <c r="H16" s="6"/>
+      <c r="I16" s="6">
         <v>29</v>
       </c>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10">
+      <c r="J16" s="6"/>
+      <c r="K16" s="6">
         <v>44</v>
       </c>
-      <c r="L16" s="10"/>
+      <c r="L16" s="6"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="10">
+      <c r="A17" s="6">
         <v>10</v>
       </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10">
+      <c r="B17" s="6"/>
+      <c r="C17" s="6">
         <v>71</v>
       </c>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10">
+      <c r="D17" s="6"/>
+      <c r="E17" s="6">
         <v>41</v>
       </c>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10">
+      <c r="F17" s="6"/>
+      <c r="G17" s="6">
         <v>30</v>
       </c>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10">
+      <c r="H17" s="6"/>
+      <c r="I17" s="6">
         <v>31</v>
       </c>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10">
+      <c r="J17" s="6"/>
+      <c r="K17" s="6">
         <v>40</v>
       </c>
-      <c r="L17" s="10"/>
+      <c r="L17" s="6"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9">
+      <c r="B18" s="11"/>
+      <c r="C18" s="11">
         <f>SUM(C17,C16,C15,C14,C13,C12,C11,C10,C9,C8) / 10</f>
         <v>75.400000000000006</v>
       </c>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9">
+      <c r="D18" s="11"/>
+      <c r="E18" s="11">
         <f>SUM(E17,E16,E15,E14,E13,E12,E11,E10,E9,E8)/10</f>
         <v>42.1</v>
       </c>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9">
+      <c r="F18" s="11"/>
+      <c r="G18" s="11">
         <f>SUM(G8:H17)/10</f>
         <v>33.299999999999997</v>
       </c>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9">
+      <c r="H18" s="11"/>
+      <c r="I18" s="11">
         <f>SUM(I8:J17)/10</f>
         <v>33.799999999999997</v>
       </c>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9">
+      <c r="J18" s="11"/>
+      <c r="K18" s="11">
         <f>SUM(K8:L17)/10</f>
         <v>41.6</v>
       </c>
-      <c r="L18" s="9"/>
+      <c r="L18" s="11"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8">
+      <c r="B19" s="12"/>
+      <c r="C19" s="12">
         <f>SUM(67+55)</f>
         <v>122</v>
       </c>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="13" t="s">
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="J19" s="8"/>
-      <c r="K19" s="13" t="s">
+      <c r="J19" s="12"/>
+      <c r="K19" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="L19" s="8"/>
+      <c r="L19" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="84">
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="A1:L3"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="K7:L7"/>
@@ -981,53 +1004,27 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="A1:L3"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>